<commit_message>
atualizacao 16 nov 2020
</commit_message>
<xml_diff>
--- a/Sistema-Operacional/Saidas/Dados-Postos/25424938_ponte_br_277_campo_largo.xlsx
+++ b/Sistema-Operacional/Saidas/Dados-Postos/25424938_ponte_br_277_campo_largo.xlsx
@@ -393,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -586,6 +586,20 @@
         <v>-42.3</v>
       </c>
     </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B14">
+        <v>39.08</v>
+      </c>
+      <c r="C14">
+        <v>58.37</v>
+      </c>
+      <c r="D14">
+        <v>-33.04</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -593,7 +607,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D367"/>
+  <dimension ref="A1:D382"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -5742,6 +5756,216 @@
         <v>-37.06</v>
       </c>
     </row>
+    <row r="368" spans="1:4">
+      <c r="A368" s="2">
+        <v>44136</v>
+      </c>
+      <c r="B368">
+        <v>35.12</v>
+      </c>
+      <c r="C368">
+        <v>58.37</v>
+      </c>
+      <c r="D368">
+        <v>-39.82</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4">
+      <c r="A369" s="2">
+        <v>44137</v>
+      </c>
+      <c r="B369">
+        <v>32.24</v>
+      </c>
+      <c r="C369">
+        <v>58.37</v>
+      </c>
+      <c r="D369">
+        <v>-44.76</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4">
+      <c r="A370" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B370">
+        <v>29.91</v>
+      </c>
+      <c r="C370">
+        <v>58.37</v>
+      </c>
+      <c r="D370">
+        <v>-48.76</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4">
+      <c r="A371" s="2">
+        <v>44139</v>
+      </c>
+      <c r="B371">
+        <v>30.42</v>
+      </c>
+      <c r="C371">
+        <v>58.37</v>
+      </c>
+      <c r="D371">
+        <v>-47.89</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4">
+      <c r="A372" s="2">
+        <v>44140</v>
+      </c>
+      <c r="B372">
+        <v>30.2</v>
+      </c>
+      <c r="C372">
+        <v>58.37</v>
+      </c>
+      <c r="D372">
+        <v>-48.26</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4">
+      <c r="A373" s="2">
+        <v>44141</v>
+      </c>
+      <c r="B373">
+        <v>28.71</v>
+      </c>
+      <c r="C373">
+        <v>58.37</v>
+      </c>
+      <c r="D373">
+        <v>-50.81</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4">
+      <c r="A374" s="2">
+        <v>44142</v>
+      </c>
+      <c r="B374">
+        <v>28.45</v>
+      </c>
+      <c r="C374">
+        <v>58.37</v>
+      </c>
+      <c r="D374">
+        <v>-51.26</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4">
+      <c r="A375" s="2">
+        <v>44143</v>
+      </c>
+      <c r="B375">
+        <v>28.03</v>
+      </c>
+      <c r="C375">
+        <v>58.37</v>
+      </c>
+      <c r="D375">
+        <v>-51.97</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4">
+      <c r="A376" s="2">
+        <v>44144</v>
+      </c>
+      <c r="B376">
+        <v>27.41</v>
+      </c>
+      <c r="C376">
+        <v>58.37</v>
+      </c>
+      <c r="D376">
+        <v>-53.04</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4">
+      <c r="A377" s="2">
+        <v>44145</v>
+      </c>
+      <c r="B377">
+        <v>27.84</v>
+      </c>
+      <c r="C377">
+        <v>58.37</v>
+      </c>
+      <c r="D377">
+        <v>-52.29</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4">
+      <c r="A378" s="2">
+        <v>44146</v>
+      </c>
+      <c r="B378">
+        <v>82.05</v>
+      </c>
+      <c r="C378">
+        <v>58.37</v>
+      </c>
+      <c r="D378">
+        <v>40.58</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4">
+      <c r="A379" s="2">
+        <v>44147</v>
+      </c>
+      <c r="B379">
+        <v>65.67</v>
+      </c>
+      <c r="C379">
+        <v>58.37</v>
+      </c>
+      <c r="D379">
+        <v>12.51</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4">
+      <c r="A380" s="2">
+        <v>44148</v>
+      </c>
+      <c r="B380">
+        <v>49.65</v>
+      </c>
+      <c r="C380">
+        <v>58.37</v>
+      </c>
+      <c r="D380">
+        <v>-14.94</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4">
+      <c r="A381" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B381">
+        <v>50.31</v>
+      </c>
+      <c r="C381">
+        <v>58.37</v>
+      </c>
+      <c r="D381">
+        <v>-13.8</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4">
+      <c r="A382" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B382">
+        <v>40.2</v>
+      </c>
+      <c r="C382">
+        <v>58.37</v>
+      </c>
+      <c r="D382">
+        <v>-31.13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>